<commit_message>
docs : update reports
</commit_message>
<xml_diff>
--- a/data/proof-of-work.xlsx
+++ b/data/proof-of-work.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://postechackr-my.sharepoint.com/personal/seungjunoh_postech_ac_kr/Documents/바탕 화면/git/Basten1209.github.io/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="11_AD4D066CA252ABDACC10481411A76B9749B8DF56" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF70C973-FD98-476A-9F1D-9C0AAE023CC0}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="11_AD4D066CA252ABDACC10481411A76B9749B8DF56" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2E5106B-434F-4D2A-AEB0-E2B6BC39C4D1}"/>
   <bookViews>
     <workbookView xWindow="5610" yWindow="2190" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Column</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -50,7 +50,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>aaaa</t>
+    <t>to be continue….</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -383,7 +383,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -409,15 +409,6 @@
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
docs : update xlsx file
</commit_message>
<xml_diff>
--- a/data/proof-of-work.xlsx
+++ b/data/proof-of-work.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://postechackr-my.sharepoint.com/personal/seungjunoh_postech_ac_kr/Documents/바탕 화면/git/Basten1209.github.io/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="482" documentId="11_AD4D066CA252ABDACC10481411A76B9749B8DF56" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B573EC95-3ED7-42BE-A929-3C3BE95151A6}"/>
+  <xr:revisionPtr revIDLastSave="567" documentId="11_AD4D066CA252ABDACC10481411A76B9749B8DF56" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58FB1AD7-BC57-40FC-9A22-2907177F8928}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$E$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,17 +28,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="143">
   <si>
     <t>Tags</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Contents</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ref</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -491,11 +487,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>POSTECH
-WorldQuant</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Won a Korea 3rd Prize in 2025 WorldQuant IQC</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -521,10 +512,6 @@
   </si>
   <si>
     <t xml:space="preserve">joined in "Startup Village Seoul" as Event Operations Part-Time Staff </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Last Update : 2025.11.14.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -538,6 +525,101 @@
   </si>
   <si>
     <t>Undergraduate Researcher in FBDA Lab(Financial Big Data Analysis Lab)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Crypto</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.06.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Certification
+Finance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POSTECH
+WorldQuant
+Finance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>투자자산운용사 취득</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Medium</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>재경관리사 취득</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.10.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.04.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자산관리사(FP) 취득</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.07.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>외환전문역 I종 취득</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.09.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정보처리산업기사 취득</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.12.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SQLD (SQL 개발자) 취득</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADsP (데이터분석 준전문가) 취득</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024.08.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비서 1급 취득</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>워드프로세서 취득</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Certification</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Low</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -545,7 +627,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -558,14 +640,6 @@
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="맑은 고딕"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -586,20 +660,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
-    <cellStyle name="하이퍼링크" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -881,10 +952,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F53"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -893,132 +964,143 @@
     <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="84.875" customWidth="1"/>
-    <col min="5" max="5" width="8.25" customWidth="1"/>
-    <col min="8" max="8" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>119</v>
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>6</v>
+        <v>55</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F4" t="s">
-        <v>8</v>
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F5" t="s">
-        <v>8</v>
+        <v>82</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="F6" t="s">
-        <v>8</v>
+        <v>27</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" t="s">
-        <v>8</v>
+        <v>42</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" t="s">
-        <v>8</v>
+        <v>78</v>
+      </c>
+      <c r="E8" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1029,747 +1111,957 @@
         <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F9" t="s">
-        <v>90</v>
+      <c r="E9" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F10" t="s">
-        <v>8</v>
+        <v>43</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>44</v>
+        <v>59</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
       </c>
       <c r="F11" t="s">
-        <v>8</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>4</v>
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F12" t="s">
-        <v>7</v>
+        <v>34</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13" t="s">
-        <v>7</v>
+      <c r="E13" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" t="s">
-        <v>3</v>
+        <v>23</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
+      </c>
+      <c r="E14" t="s">
+        <v>7</v>
       </c>
       <c r="F14" t="s">
-        <v>6</v>
+        <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>26</v>
+        <v>35</v>
+      </c>
+      <c r="E15" t="s">
+        <v>89</v>
       </c>
       <c r="F15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
         <v>24</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>36</v>
+        <v>26</v>
+      </c>
+      <c r="E16" t="s">
+        <v>6</v>
       </c>
       <c r="F16" t="s">
-        <v>90</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>98</v>
-      </c>
       <c r="D18" s="1" t="s">
-        <v>59</v>
+        <v>29</v>
+      </c>
+      <c r="E18" t="s">
+        <v>6</v>
       </c>
       <c r="F18" t="s">
-        <v>6</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>111</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>111</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>30</v>
       </c>
-      <c r="F19" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>113</v>
-      </c>
       <c r="B20" t="s">
-        <v>113</v>
+        <v>30</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>115</v>
+        <v>31</v>
+      </c>
+      <c r="E20" t="s">
+        <v>6</v>
       </c>
       <c r="F20" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>96</v>
+        <v>3</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>32</v>
+        <v>60</v>
+      </c>
+      <c r="E21" t="s">
+        <v>6</v>
       </c>
       <c r="F21" t="s">
-        <v>7</v>
+        <v>121</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>4</v>
+        <v>95</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>61</v>
+        <v>40</v>
+      </c>
+      <c r="E22" t="s">
+        <v>6</v>
       </c>
       <c r="F22" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>96</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E23" s="2"/>
+        <v>33</v>
+      </c>
+      <c r="E23" t="s">
+        <v>5</v>
+      </c>
       <c r="F23" t="s">
-        <v>7</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
+      </c>
+      <c r="E24" t="s">
+        <v>5</v>
       </c>
       <c r="F24" t="s">
-        <v>6</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
+      </c>
+      <c r="E25" t="s">
+        <v>6</v>
       </c>
       <c r="F25" t="s">
-        <v>6</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>97</v>
+        <v>69</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
+      </c>
+      <c r="E26" t="s">
+        <v>7</v>
       </c>
       <c r="F26" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>70</v>
+        <v>15</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F27" t="s">
-        <v>8</v>
+        <v>45</v>
+      </c>
+      <c r="E27" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="B28" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F28" t="s">
+        <v>49</v>
+      </c>
+      <c r="E28" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" t="s">
         <v>47</v>
       </c>
-      <c r="B29" t="s">
-        <v>48</v>
-      </c>
       <c r="C29" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F29" t="s">
-        <v>8</v>
+        <v>51</v>
+      </c>
+      <c r="E29" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>51</v>
-      </c>
-      <c r="B30" t="s">
-        <v>48</v>
+        <v>135</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>16</v>
+        <v>141</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F30" t="s">
-        <v>8</v>
+        <v>136</v>
+      </c>
+      <c r="E30" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+      <c r="E31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>54</v>
-      </c>
-      <c r="B32" t="s">
-        <v>45</v>
+        <v>129</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>16</v>
+        <v>123</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F32" t="s">
+        <v>130</v>
+      </c>
+      <c r="E32" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>57</v>
+        <v>122</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>4</v>
+        <v>123</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F33" t="s">
-        <v>6</v>
+        <v>125</v>
+      </c>
+      <c r="E33" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>57</v>
-      </c>
-      <c r="B34" t="s">
-        <v>62</v>
+        <v>131</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>63</v>
+        <v>123</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F34" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+      <c r="E34" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="B35" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F35" t="s">
-        <v>7</v>
+        <v>54</v>
+      </c>
+      <c r="E35" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>138</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E36" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>138</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E37" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>133</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E38" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>133</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E39" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>128</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E40" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>56</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E41" t="s">
+        <v>5</v>
+      </c>
+      <c r="F41" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>56</v>
+      </c>
+      <c r="B42" t="s">
+        <v>61</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E42" t="s">
+        <v>6</v>
+      </c>
+      <c r="F42" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>70</v>
+      </c>
+      <c r="B43" t="s">
+        <v>68</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E43" t="s">
+        <v>6</v>
+      </c>
+      <c r="F43" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>70</v>
+      </c>
+      <c r="B44" t="s">
         <v>71</v>
       </c>
-      <c r="B36" t="s">
-        <v>72</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F36" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>68</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F37" t="s">
+      <c r="C44" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E44" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>109</v>
-      </c>
-      <c r="B38" t="s">
-        <v>110</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F38" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>104</v>
-      </c>
-      <c r="B39" t="s">
-        <v>104</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F39" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>72</v>
-      </c>
-      <c r="B40" t="s">
-        <v>72</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F40" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>120</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="F41" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>62</v>
-      </c>
-      <c r="B42" t="s">
-        <v>62</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F42" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>62</v>
-      </c>
-      <c r="B43" t="s">
-        <v>62</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F43" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>62</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="F44" t="s">
-        <v>90</v>
+        <v>121</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="E45" t="s">
+        <v>6</v>
+      </c>
       <c r="F45" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>108</v>
+      </c>
+      <c r="B46" t="s">
+        <v>109</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E46" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>103</v>
+      </c>
+      <c r="B47" t="s">
+        <v>103</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E47" t="s">
+        <v>6</v>
+      </c>
+      <c r="F47" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>71</v>
+      </c>
+      <c r="B48" t="s">
+        <v>71</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E48" t="s">
+        <v>90</v>
+      </c>
+      <c r="F48" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>117</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E49" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>64</v>
-      </c>
-      <c r="B46" t="s">
-        <v>64</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F46" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>89</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F47" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="33" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>89</v>
-      </c>
-      <c r="B48" t="s">
-        <v>89</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="F48" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>89</v>
-      </c>
-      <c r="B49" t="s">
-        <v>89</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>118</v>
-      </c>
       <c r="F49" t="s">
-        <v>90</v>
+        <v>121</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
+        <v>61</v>
+      </c>
+      <c r="B50" t="s">
+        <v>61</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E50" t="s">
         <v>89</v>
       </c>
-      <c r="B50" t="s">
+      <c r="F50" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>61</v>
+      </c>
+      <c r="B51" t="s">
+        <v>61</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E51" t="s">
+        <v>90</v>
+      </c>
+      <c r="F51" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>61</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E52" t="s">
         <v>89</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F50" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>89</v>
-      </c>
-      <c r="B51" t="s">
-        <v>89</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F51" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>93</v>
-      </c>
-      <c r="B52" t="s">
-        <v>93</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="F52" t="s">
-        <v>90</v>
+        <v>121</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="33" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
+        <v>63</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E53" t="s">
+        <v>90</v>
+      </c>
+      <c r="F53" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>63</v>
+      </c>
+      <c r="B54" t="s">
+        <v>63</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E54" t="s">
+        <v>89</v>
+      </c>
+      <c r="F54" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>88</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E55" t="s">
+        <v>89</v>
+      </c>
+      <c r="F55" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>88</v>
+      </c>
+      <c r="B56" t="s">
+        <v>88</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E56" t="s">
+        <v>89</v>
+      </c>
+      <c r="F56" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>88</v>
+      </c>
+      <c r="B57" t="s">
+        <v>88</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E57" t="s">
+        <v>89</v>
+      </c>
+      <c r="F57" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>88</v>
+      </c>
+      <c r="B58" t="s">
+        <v>88</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E58" t="s">
+        <v>89</v>
+      </c>
+      <c r="F58" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>88</v>
+      </c>
+      <c r="B59" t="s">
+        <v>88</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E59" t="s">
+        <v>91</v>
+      </c>
+      <c r="F59" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>92</v>
+      </c>
+      <c r="B60" t="s">
+        <v>92</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B53" t="s">
-        <v>105</v>
-      </c>
-      <c r="C53" s="1" t="s">
+      <c r="E60" t="s">
+        <v>89</v>
+      </c>
+      <c r="F60" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>104</v>
+      </c>
+      <c r="B61" t="s">
+        <v>104</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D53" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F53" t="s">
-        <v>92</v>
+      <c r="E61" t="s">
+        <v>91</v>
+      </c>
+      <c r="F61" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:E2" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:E53">
-      <sortCondition ref="A2"/>
+  <autoFilter ref="A1:F1" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F61">
+      <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>